<commit_message>
fix: delete useless folders/files
</commit_message>
<xml_diff>
--- a/source_files/comp_scenario.xlsx
+++ b/source_files/comp_scenario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="127">
   <si>
     <t xml:space="preserve">TransactionID</t>
   </si>
@@ -1068,8 +1068,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2285,68 +2285,8 @@
         <v>247.5</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="3" t="n">
-        <v>43859</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="5" t="n">
-        <v>75</v>
-      </c>
-      <c r="F40" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="7" t="n">
-        <f aca="false">IF(G40="Y",(0.1*E40*F40),0)</f>
-        <v>22.5</v>
-      </c>
-      <c r="I40" s="5" t="n">
-        <f aca="false">(E40*F40)+H40</f>
-        <v>247.5</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="3" t="n">
-        <v>44072</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="5" t="n">
-        <v>75</v>
-      </c>
-      <c r="F41" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="7" t="n">
-        <f aca="false">IF(G41="Y",(0.1*E41*F41),0)</f>
-        <v>22.5</v>
-      </c>
-      <c r="I41" s="5" t="n">
-        <f aca="false">(E41*F41)+H41</f>
-        <v>247.5</v>
-      </c>
-    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3283,8 +3223,8 @@
     <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3371,7 +3311,7 @@
   </sheetPr>
   <dimension ref="B1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -35025,7 +34965,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>